<commit_message>
Add stock info for following keys: TXN,ULVR.L,VZ,HEN3.DE,MPW,BA,HL.L,TIP,MCHP,ITW,TLT,KR,AMAT,XLV,NXPI,BPY,GRMN,ATVI,CME,AGN.
</commit_message>
<xml_diff>
--- a/Naslovi_info.xlsx
+++ b/Naslovi_info.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damird/Osebno/IB_to_eDavki/2020/eToro/ddeze-etoro-edavki/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7C20C4-5415-DC4C-BCB3-549FE05853DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Info" sheetId="1" r:id="rId4"/>
+    <sheet name="Info" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="550">
   <si>
     <t>Symbol</t>
   </si>
@@ -1418,50 +1427,313 @@
   </si>
   <si>
     <t>Bethesda, Maryland, United States</t>
+  </si>
+  <si>
+    <t>TXN</t>
+  </si>
+  <si>
+    <t>ULVR.L</t>
+  </si>
+  <si>
+    <t>VZ</t>
+  </si>
+  <si>
+    <t>HEN3.DE</t>
+  </si>
+  <si>
+    <t>MPW</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>HL.L</t>
+  </si>
+  <si>
+    <t>TIP</t>
+  </si>
+  <si>
+    <t>MCHP</t>
+  </si>
+  <si>
+    <t>ITW</t>
+  </si>
+  <si>
+    <t>TLT</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>AMAT</t>
+  </si>
+  <si>
+    <t>XLV</t>
+  </si>
+  <si>
+    <t>AGN</t>
+  </si>
+  <si>
+    <t>NXPI</t>
+  </si>
+  <si>
+    <t>BPY</t>
+  </si>
+  <si>
+    <t>GRMN</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
+    <t>CME</t>
+  </si>
+  <si>
+    <t>Texas Instruments Incorporated</t>
+  </si>
+  <si>
+    <t>12500 TI Boulevard Dallas, TX 75243 United States</t>
+  </si>
+  <si>
+    <t>US8825081040</t>
+  </si>
+  <si>
+    <t>Unilever PLC</t>
+  </si>
+  <si>
+    <t>Unilever House 100 Victoria Embankment London EC4Y 0DY United Kingdom</t>
+  </si>
+  <si>
+    <t>GB00B10RZP78</t>
+  </si>
+  <si>
+    <t>Verizon Communications Inc.</t>
+  </si>
+  <si>
+    <t>1095 Avenue of the Americas, New York, NY 10036</t>
+  </si>
+  <si>
+    <t>US92343V1044</t>
+  </si>
+  <si>
+    <t>Henkel AG &amp; Co. KGaA</t>
+  </si>
+  <si>
+    <t>DE0006048408</t>
+  </si>
+  <si>
+    <t>Henkelstrasse 67, Düsseldorf 40589, Germany</t>
+  </si>
+  <si>
+    <t>Medical Properties Trust, Inc.</t>
+  </si>
+  <si>
+    <t>1000 Urban Center Drive, Suite 501, Birmingham, AL 35242, United States</t>
+  </si>
+  <si>
+    <t>US58463J3041</t>
+  </si>
+  <si>
+    <t>The Boeing Company</t>
+  </si>
+  <si>
+    <t>100 North Riverside Plaza, Chicago, IL 60606-1596, United States</t>
+  </si>
+  <si>
+    <t>US0970231058</t>
+  </si>
+  <si>
+    <t>Hargreaves Lansdown plc</t>
+  </si>
+  <si>
+    <t>One College Square South, Anchor Road, Bristol BS1 5HL, United Kingdom</t>
+  </si>
+  <si>
+    <t>GB00B1VZ0M25</t>
+  </si>
+  <si>
+    <t>iShares TIPS Bond ETF</t>
+  </si>
+  <si>
+    <t>US4642871762</t>
+  </si>
+  <si>
+    <t>iShares</t>
+  </si>
+  <si>
+    <t>Microchip Technology Incorporated</t>
+  </si>
+  <si>
+    <t>2355 West Chandler Boulevard, Chandler, AZ 85224-6199, United States</t>
+  </si>
+  <si>
+    <t>US5950171042</t>
+  </si>
+  <si>
+    <t>Illinois Tool Works Inc.</t>
+  </si>
+  <si>
+    <t>155 Harlem Avenue, Glenview, IL 60025-4075, United States</t>
+  </si>
+  <si>
+    <t>US4523081093</t>
+  </si>
+  <si>
+    <t>iShares 20+ Year Treasury Bond ETF</t>
+  </si>
+  <si>
+    <t>US4642874329</t>
+  </si>
+  <si>
+    <t>The Kroger Co.</t>
+  </si>
+  <si>
+    <t>1014 Vine Street, Cincinnati, OH 45202, United States</t>
+  </si>
+  <si>
+    <t>US501044DN88</t>
+  </si>
+  <si>
+    <t>Applied Materials, Inc.</t>
+  </si>
+  <si>
+    <t>3050 Bowers Avenue, PO Box 58039, Santa Clara, CA 95052-3299, United States</t>
+  </si>
+  <si>
+    <t>US0382221051</t>
+  </si>
+  <si>
+    <t>Health Care Select Sector SPDR Fund</t>
+  </si>
+  <si>
+    <t>US81369Y2090</t>
+  </si>
+  <si>
+    <t>SPDR State Street Global Advisors</t>
+  </si>
+  <si>
+    <t>NXP Semiconductors N.V.</t>
+  </si>
+  <si>
+    <t>High Tech Campus 60, Eindhoven 5656 AG, Netherlands</t>
+  </si>
+  <si>
+    <t>NL0009538784</t>
+  </si>
+  <si>
+    <t>Brookfield Property Partners L.P.</t>
+  </si>
+  <si>
+    <t>73 Front Street, 5th Floor, Hamilton HM 12, Bermuda</t>
+  </si>
+  <si>
+    <t>BMG162491077</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>Garmin Ltd.</t>
+  </si>
+  <si>
+    <t>Mühlentalstrasse 2, Schaffhausen 8200, Switzerland</t>
+  </si>
+  <si>
+    <t>CH0114405324</t>
+  </si>
+  <si>
+    <t>Activision Blizzard, Inc.</t>
+  </si>
+  <si>
+    <t>3100 Ocean Park Boulevard, Santa Monica, CA 90405, United States</t>
+  </si>
+  <si>
+    <t>US00507V1098</t>
+  </si>
+  <si>
+    <t>CME Group Inc.</t>
+  </si>
+  <si>
+    <t>20 South Wacker Drive, Chicago, IL 60606, United States</t>
+  </si>
+  <si>
+    <t>US12572Q1058</t>
+  </si>
+  <si>
+    <t>Algernon Pharmaceuticals Inc.</t>
+  </si>
+  <si>
+    <t>700 West Pender Street, Suite 915, Vancouver, BC V6C 1G8, Canada</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CA01559R1038</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Bwhaasgrotesk-55roman-web"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1469,112 +1741,103 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEEAF6"/>
+          <bgColor rgb="FFDEEAF6"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FFD8D8D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="5"/>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD8D8D8"/>
-          <bgColor rgb="FFD8D8D8"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Info-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Info-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E117" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E137">
   <tableColumns count="5">
-    <tableColumn name="Symbol" id="1"/>
-    <tableColumn name="ISIN" id="2"/>
-    <tableColumn name="Name" id="3"/>
-    <tableColumn name="Address" id="4"/>
-    <tableColumn name="CountryCode" id="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ISIN"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Address"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CountryCode"/>
   </tableColumns>
-  <tableStyleInfo name="Info-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Info-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1764,28 +2027,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E962"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.5"/>
-    <col customWidth="1" min="2" max="2" width="15.0"/>
-    <col customWidth="1" min="3" max="3" width="35.0"/>
-    <col customWidth="1" min="4" max="4" width="103.13"/>
-    <col customWidth="1" min="5" max="5" width="12.75"/>
-    <col customWidth="1" min="6" max="26" width="7.63"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="103.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1802,7 +2065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1819,7 +2082,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1836,7 +2099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1853,7 +2116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1870,7 +2133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1887,7 +2150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1904,7 +2167,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1921,7 +2184,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1938,7 +2201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -1955,7 +2218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1972,7 +2235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1989,7 +2252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -2006,7 +2269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -2023,7 +2286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
@@ -2040,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -2057,7 +2320,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>68</v>
       </c>
@@ -2074,7 +2337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
@@ -2091,7 +2354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
@@ -2108,7 +2371,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -2125,7 +2388,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>84</v>
       </c>
@@ -2142,7 +2405,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
@@ -2159,7 +2422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>92</v>
       </c>
@@ -2176,7 +2439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>96</v>
       </c>
@@ -2193,7 +2456,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>100</v>
       </c>
@@ -2210,7 +2473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -2227,7 +2490,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>108</v>
       </c>
@@ -2244,7 +2507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>112</v>
       </c>
@@ -2261,7 +2524,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>116</v>
       </c>
@@ -2278,7 +2541,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>120</v>
       </c>
@@ -2295,7 +2558,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>124</v>
       </c>
@@ -2312,7 +2575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>128</v>
       </c>
@@ -2329,7 +2592,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>132</v>
       </c>
@@ -2346,7 +2609,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>136</v>
       </c>
@@ -2363,7 +2626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
@@ -2380,7 +2643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>144</v>
       </c>
@@ -2397,7 +2660,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>149</v>
       </c>
@@ -2414,7 +2677,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>153</v>
       </c>
@@ -2431,7 +2694,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>157</v>
       </c>
@@ -2448,7 +2711,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>162</v>
       </c>
@@ -2465,7 +2728,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>167</v>
       </c>
@@ -2482,7 +2745,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>171</v>
       </c>
@@ -2499,7 +2762,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>175</v>
       </c>
@@ -2516,7 +2779,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>178</v>
       </c>
@@ -2533,7 +2796,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>183</v>
       </c>
@@ -2550,7 +2813,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>188</v>
       </c>
@@ -2567,7 +2830,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>192</v>
       </c>
@@ -2584,7 +2847,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>196</v>
       </c>
@@ -2601,7 +2864,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>200</v>
       </c>
@@ -2618,7 +2881,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>204</v>
       </c>
@@ -2635,7 +2898,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>208</v>
       </c>
@@ -2652,7 +2915,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>212</v>
       </c>
@@ -2669,7 +2932,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>216</v>
       </c>
@@ -2686,7 +2949,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>220</v>
       </c>
@@ -2703,7 +2966,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="1:5" ht="15.75" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>224</v>
       </c>
@@ -2720,7 +2983,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:5" ht="15.75" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>227</v>
       </c>
@@ -2737,7 +3000,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>231</v>
       </c>
@@ -2754,7 +3017,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:5" ht="15.75" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>235</v>
       </c>
@@ -2771,7 +3034,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="1:5" ht="15.75" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>239</v>
       </c>
@@ -2788,7 +3051,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:5" ht="15.75" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>243</v>
       </c>
@@ -2805,7 +3068,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>247</v>
       </c>
@@ -2822,7 +3085,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>251</v>
       </c>
@@ -2839,7 +3102,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>254</v>
       </c>
@@ -2856,7 +3119,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1">
       <c r="A64" s="2" t="s">
         <v>258</v>
       </c>
@@ -2873,7 +3136,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>262</v>
       </c>
@@ -2890,7 +3153,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>266</v>
       </c>
@@ -2907,7 +3170,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>270</v>
       </c>
@@ -2924,7 +3187,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1">
       <c r="A68" s="2" t="s">
         <v>274</v>
       </c>
@@ -2941,7 +3204,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>278</v>
       </c>
@@ -2958,7 +3221,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>282</v>
       </c>
@@ -2975,7 +3238,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>286</v>
       </c>
@@ -2992,7 +3255,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>290</v>
       </c>
@@ -3009,7 +3272,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>294</v>
       </c>
@@ -3026,7 +3289,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>297</v>
       </c>
@@ -3043,7 +3306,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>299</v>
       </c>
@@ -3060,7 +3323,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>303</v>
       </c>
@@ -3077,7 +3340,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>307</v>
       </c>
@@ -3094,7 +3357,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>310</v>
       </c>
@@ -3111,7 +3374,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>314</v>
       </c>
@@ -3128,7 +3391,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>318</v>
       </c>
@@ -3145,7 +3408,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>321</v>
       </c>
@@ -3162,7 +3425,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:5" ht="15.75" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>325</v>
       </c>
@@ -3179,7 +3442,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:5" ht="15.75" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>329</v>
       </c>
@@ -3196,7 +3459,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:5" ht="15.75" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>333</v>
       </c>
@@ -3213,7 +3476,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:5" ht="15.75" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>337</v>
       </c>
@@ -3230,7 +3493,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:5" ht="15.75" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>340</v>
       </c>
@@ -3247,7 +3510,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:5" ht="15.75" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>344</v>
       </c>
@@ -3264,7 +3527,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:5" ht="15.75" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>348</v>
       </c>
@@ -3281,7 +3544,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:5" ht="15.75" customHeight="1">
       <c r="A89" s="2" t="s">
         <v>352</v>
       </c>
@@ -3298,7 +3561,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:5" ht="15.75" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>356</v>
       </c>
@@ -3315,7 +3578,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:5" ht="15.75" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>359</v>
       </c>
@@ -3332,7 +3595,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:5" ht="15.75" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>363</v>
       </c>
@@ -3349,7 +3612,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:5" ht="15.75" customHeight="1">
       <c r="A93" s="6" t="s">
         <v>367</v>
       </c>
@@ -3366,7 +3629,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:5" ht="15.75" customHeight="1">
       <c r="A94" s="6" t="s">
         <v>372</v>
       </c>
@@ -3383,7 +3646,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:5" ht="15.75" customHeight="1">
       <c r="A95" s="6" t="s">
         <v>377</v>
       </c>
@@ -3400,7 +3663,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:5" ht="15.75" customHeight="1">
       <c r="A96" s="6" t="s">
         <v>381</v>
       </c>
@@ -3417,7 +3680,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1">
       <c r="A97" s="6" t="s">
         <v>385</v>
       </c>
@@ -3434,7 +3697,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1">
       <c r="A98" s="6" t="s">
         <v>389</v>
       </c>
@@ -3451,7 +3714,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1">
       <c r="A99" s="6" t="s">
         <v>393</v>
       </c>
@@ -3468,7 +3731,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1">
       <c r="A100" s="6" t="s">
         <v>397</v>
       </c>
@@ -3485,7 +3748,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1">
       <c r="A101" s="6" t="s">
         <v>401</v>
       </c>
@@ -3502,7 +3765,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="1:5" ht="15.75" customHeight="1">
       <c r="A102" s="6" t="s">
         <v>405</v>
       </c>
@@ -3519,7 +3782,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="1:5" ht="15.75" customHeight="1">
       <c r="A103" s="6" t="s">
         <v>409</v>
       </c>
@@ -3536,7 +3799,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="1:5" ht="15.75" customHeight="1">
       <c r="A104" s="8" t="s">
         <v>413</v>
       </c>
@@ -3553,7 +3816,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="1:5" ht="15.75" customHeight="1">
       <c r="A105" s="6" t="s">
         <v>417</v>
       </c>
@@ -3570,7 +3833,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="1:5" ht="15.75" customHeight="1">
       <c r="A106" s="8" t="s">
         <v>421</v>
       </c>
@@ -3587,7 +3850,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1">
       <c r="A107" s="6" t="s">
         <v>425</v>
       </c>
@@ -3604,7 +3867,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="1:5" ht="15.75" customHeight="1">
       <c r="A108" s="6" t="s">
         <v>429</v>
       </c>
@@ -3621,7 +3884,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1">
       <c r="A109" s="9" t="s">
         <v>433</v>
       </c>
@@ -3638,7 +3901,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1">
       <c r="A110" s="6" t="s">
         <v>437</v>
       </c>
@@ -3655,7 +3918,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1">
       <c r="A111" s="6" t="s">
         <v>441</v>
       </c>
@@ -3672,7 +3935,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1">
       <c r="A112" s="8" t="s">
         <v>445</v>
       </c>
@@ -3689,7 +3952,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="1:5" ht="15.75" customHeight="1">
       <c r="A113" s="6" t="s">
         <v>450</v>
       </c>
@@ -3706,7 +3969,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="1:5" ht="15.75" customHeight="1">
       <c r="A114" s="6" t="s">
         <v>453</v>
       </c>
@@ -3723,7 +3986,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="1:5" ht="15.75" customHeight="1">
       <c r="A115" s="6" t="s">
         <v>457</v>
       </c>
@@ -3740,7 +4003,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="1:5" ht="15.75" customHeight="1">
       <c r="A116" s="8" t="s">
         <v>461</v>
       </c>
@@ -3757,7 +4020,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="1:5" ht="15.75" customHeight="1">
       <c r="A117" s="6" t="s">
         <v>465</v>
       </c>
@@ -3767,40 +4030,360 @@
       <c r="C117" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="D117" s="6" t="s">
+      <c r="D117" s="10" t="s">
         <v>468</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="118" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A118" t="s">
+        <v>469</v>
+      </c>
+      <c r="B118" t="s">
+        <v>491</v>
+      </c>
+      <c r="C118" t="s">
+        <v>489</v>
+      </c>
+      <c r="D118" t="s">
+        <v>490</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A119" t="s">
+        <v>470</v>
+      </c>
+      <c r="B119" t="s">
+        <v>494</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="D119" t="s">
+        <v>493</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A120" t="s">
+        <v>471</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C120" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A121" t="s">
+        <v>472</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A122" t="s">
+        <v>473</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A123" t="s">
+        <v>474</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A124" t="s">
+        <v>475</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A125" t="s">
+        <v>476</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A126" t="s">
+        <v>477</v>
+      </c>
+      <c r="B126" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="D126" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A127" t="s">
+        <v>478</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="D127" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A128" t="s">
+        <v>479</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A129" t="s">
+        <v>480</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="C129" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A130" t="s">
+        <v>481</v>
+      </c>
+      <c r="B130" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="E130" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A131" t="s">
+        <v>482</v>
+      </c>
+      <c r="B131" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="C131" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="D131" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="E131" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A132" t="s">
+        <v>484</v>
+      </c>
+      <c r="B132" s="11" t="s">
+        <v>532</v>
+      </c>
+      <c r="C132" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="D132" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A133" t="s">
+        <v>485</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="C133" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="E133" s="7" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A134" t="s">
+        <v>486</v>
+      </c>
+      <c r="B134" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="C134" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="D134" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="E134" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A135" t="s">
+        <v>487</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="C135" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="D135" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A136" t="s">
+        <v>488</v>
+      </c>
+      <c r="B136" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="C136" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A137" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="B137" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="139" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="140" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="141" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="142" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="143" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="144" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1"/>
     <row r="146" ht="15.75" customHeight="1"/>
     <row r="147" ht="15.75" customHeight="1"/>
@@ -4619,22 +5202,18 @@
     <row r="960" ht="15.75" customHeight="1"/>
     <row r="961" ht="15.75" customHeight="1"/>
     <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A104"/>
-    <hyperlink r:id="rId2" ref="A106"/>
-    <hyperlink r:id="rId3" ref="A109"/>
-    <hyperlink r:id="rId4" ref="A112"/>
-    <hyperlink r:id="rId5" ref="A116"/>
+    <hyperlink ref="A104" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A106" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A109" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A112" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A116" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>